<commit_message>
Added Bug_reports.pdf - file with all found bugs described. updated English_levels.xlsx - file with mindpap, EC and check-list
</commit_message>
<xml_diff>
--- a/English_levels/English_levels.xlsx
+++ b/English_levels/English_levels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newak\OneDrive\Рабочий стол\Bonzik\QA_cases\English_levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819469DC-F633-41DE-8428-12C81A017A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC2C879-0AD4-4BE0-A29C-BB5F3DFF673C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="-11520" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="-11520" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Чек-лист" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="125">
   <si>
     <t>Passed</t>
   </si>
@@ -217,15 +217,9 @@
     <t>Убедиться, что сайт не даёт заполнить поле значением "-0.5"</t>
   </si>
   <si>
-    <t>Убедиться, что при заполнении поля значением "0" на следующем экране выводится результат "А1"</t>
-  </si>
-  <si>
     <t>Убедиться, что сайт не даёт заполнить поле значением "-5"</t>
   </si>
   <si>
-    <t>Убедиться, что при заполнении поля значением "0.5" на следующем экране выводится результат "А1"</t>
-  </si>
-  <si>
     <t>Числа от 0 до 2.5</t>
   </si>
   <si>
@@ -244,9 +238,6 @@
     <t>Числа от 8.5 до 9</t>
   </si>
   <si>
-    <t>Для того, чтобы удостовериться, что сайт допускает к расчётам только валидные данные</t>
-  </si>
-  <si>
     <t>Для того, чтобы удостовериться, что сайт правильно ощущает валидный диапазон бальной шкалы</t>
   </si>
   <si>
@@ -298,57 +289,6 @@
     <t>Для того, чтобы убедиться, что сайт правильно выставляет соответствие уровня баллам</t>
   </si>
   <si>
-    <t>Убедиться, что при заполнении поля значением "1" на следующем экране выводится результат "А1"</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "1.5" на следующем экране выводится результат "А1"</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "2" на следующем экране выводится результат "А1"</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "2.5" на следующем экране выводится результат "А1"</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "3" на следующем экране выводится результат "А2"</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "3.5" на следующем экране выводится результат "А2"</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "4" на следующем экране выводится результат "В1"</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "4.5" на следующем экране выводится результат "В1"</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "5" на следующем экране выводится результат "В1"</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "5.5" на следующем экране выводится результат "В2"</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "6" на следующем экране выводится результат "В2"</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "6.5" на следующем экране выводится результат "В2"</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "7" на следующем экране выводится результат "С1"</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "7.5" на следующем экране выводится результат "С1"</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "8" на следующем экране выводится результат "С1"</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "8.5" на следующем экране выводится результат "С2"</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "9" на следующем экране выводится результат "С2"</t>
-  </si>
-  <si>
     <t>Убедиться, что при заполнении поля значением "9.5" сайт даёт понять, что это невалидное число</t>
   </si>
   <si>
@@ -358,23 +298,119 @@
     <t>Убедиться, что при заполнении поля значением "14" сайт даёт понять, что это невалидное число</t>
   </si>
   <si>
-    <t>Убедиться, что при заполнении поля значением "6.1" сайт даёт понять, что это невалидное число</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "6.005" сайт даёт понять, что это невалидное число</t>
-  </si>
-  <si>
-    <t>Убедиться, что при заполнении поля значением "8.999999" сайт даёт понять, что это невалидное число</t>
-  </si>
-  <si>
     <t>Сайт просит ввести валидное число и подсвечивает название поля красным. Лучше бы писал, что поле не может быть пустым.</t>
+  </si>
+  <si>
+    <t>Bug-report #1</t>
+  </si>
+  <si>
+    <t>Bug-report #2</t>
+  </si>
+  <si>
+    <t>Bug-report #3</t>
+  </si>
+  <si>
+    <t>Bug-report #4</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "6.1" сайт даёт понять, что это невалидное число (проверка на невалидность не кратных 0.5)</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "6.005" сайт даёт понять, что это невалидное число (проверка на невалидность не кратных 0.5)</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "0" на следующем экране выводится результат "А1" и картинка "А1"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "0.5" на следующем экране выводится результат "А1" и картинка "А1"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "1" на следующем экране выводится результат "А1" и картинка "А1"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "1.5" на следующем экране выводится результат "А1" и картинка "А1"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "2" на следующем экране выводится результат "А1" и картинка "А1"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "2.5" на следующем экране выводится результат "А1" и картинка "А1"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "3" на следующем экране выводится результат "А2" и картинка "А2"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "3.5" на следующем экране выводится результат "А2" и картинка "А2"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "4" на следующем экране выводится результат "В1" и картинка "В1"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "4.5" на следующем экране выводится результат "В1" и картинка "В1"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "5" на следующем экране выводится результат "В1" и картинка "В1"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "5.5" на следующем экране выводится результат "В2" и картинка "В2"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "6" на следующем экране выводится результат "В2" и картинка "В2"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "6.5" на следующем экране выводится результат "В2" и картинка "В2"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "7" на следующем экране выводится результат "С1" и картинка "С1"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "7.5" на следующем экране выводится результат "С1" и картинка "С1"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "8" на следующем экране выводится результат "С1" и картинка "С1"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "8.5" на следующем экране выводится результат "С2" и картинка "С2"</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "9" на следующем экране выводится результат "С2" и картинка "С2"</t>
+  </si>
+  <si>
+    <t>Bug-report #5</t>
+  </si>
+  <si>
+    <t>Bug-report #6</t>
+  </si>
+  <si>
+    <t>Bug-report #7</t>
+  </si>
+  <si>
+    <t>Bug-report #8</t>
+  </si>
+  <si>
+    <t>Bug-report #9</t>
+  </si>
+  <si>
+    <t>Bug-report #10</t>
+  </si>
+  <si>
+    <t>Убедиться, что при заполнении поля значением "5.999999" сайт даёт понять, что это невалидное число (проверка на невалидность не кратных 0.5)</t>
+  </si>
+  <si>
+    <t>Убедиться, что после введения в поле "Ито Хиробуми", считаемого сайтом невалидным, и последующем вводе валидного значения "5" и возвращении на главную страницу, информация об ошибке пропадает</t>
+  </si>
+  <si>
+    <t>Bug-report #11</t>
+  </si>
+  <si>
+    <t>Для того, чтобы удостовериться, что сайт допускает к расчётам только цифры и символ точки</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,6 +443,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -538,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -580,50 +622,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -695,22 +715,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>483871</xdr:colOff>
+      <xdr:colOff>217170</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>174194</xdr:rowOff>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>549094</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>72317</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2">
+        <xdr:cNvPr id="4" name="Рисунок 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{187F70E7-C7D2-A5CD-B8F1-BA7DCD3B770F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47013F0E-DE71-3FA7-C4BC-D91B84911810}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -726,8 +746,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="483871" y="174194"/>
-          <a:ext cx="11038023" cy="6664756"/>
+          <a:off x="217170" y="180974"/>
+          <a:ext cx="11746230" cy="8578143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1002,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q55"/>
+  <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1065,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
@@ -1163,7 +1183,9 @@
       <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1176,7 +1198,9 @@
       <c r="B14" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="N14" s="2"/>
       <c r="O14" s="4"/>
       <c r="P14" s="5"/>
@@ -1189,7 +1213,9 @@
       <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="6"/>
+      <c r="C15" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
@@ -1201,7 +1227,9 @@
       <c r="B16" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="6"/>
+      <c r="C16" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
@@ -1213,7 +1241,9 @@
       <c r="B17" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="6"/>
+      <c r="C17" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="N17" s="2"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
@@ -1226,7 +1256,9 @@
       <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
@@ -1238,7 +1270,9 @@
       <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="6"/>
+      <c r="C19" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="N19" s="9"/>
       <c r="O19" s="7"/>
       <c r="P19" s="3"/>
@@ -1251,7 +1285,12 @@
       <c r="B20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="21" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
@@ -1260,7 +1299,12 @@
       <c r="B21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="6"/>
+      <c r="C21" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="22" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
@@ -1269,7 +1313,12 @@
       <c r="B22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="6"/>
+      <c r="C22" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="23" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
@@ -1278,7 +1327,12 @@
       <c r="B23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="C23" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="24" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
@@ -1287,7 +1341,12 @@
       <c r="B24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="6"/>
+      <c r="C24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="25" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
@@ -1296,7 +1355,12 @@
       <c r="B25" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="6"/>
+      <c r="C25" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="26" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
@@ -1305,7 +1369,12 @@
       <c r="B26" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="6"/>
+      <c r="C26" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="27" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
@@ -1314,7 +1383,12 @@
       <c r="B27" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="6"/>
+      <c r="C27" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="28" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
@@ -1323,16 +1397,26 @@
       <c r="B28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="6"/>
+      <c r="C28" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="29" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="6"/>
+        <v>62</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="30" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
@@ -1341,346 +1425,422 @@
       <c r="B30" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="6"/>
+      <c r="C30" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="31" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="23"/>
+        <v>96</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="23"/>
-    </row>
-    <row r="33" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="23"/>
+    </row>
+    <row r="33" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="23"/>
-    </row>
-    <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="23"/>
+    </row>
+    <row r="34" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="23"/>
-    </row>
-    <row r="35" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="23"/>
+    </row>
+    <row r="35" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>34</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="23"/>
-    </row>
-    <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="23"/>
+    </row>
+    <row r="36" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="23"/>
-    </row>
-    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="23"/>
+    </row>
+    <row r="37" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>36</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="23"/>
-    </row>
-    <row r="38" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" s="9"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="23"/>
+    </row>
+    <row r="38" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="23"/>
-    </row>
-    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>115</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="23"/>
+    </row>
+    <row r="39" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>38</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="23"/>
-    </row>
-    <row r="40" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="23"/>
+    </row>
+    <row r="40" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="23"/>
-    </row>
-    <row r="41" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="23"/>
+    </row>
+    <row r="41" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>40</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="23"/>
-    </row>
-    <row r="42" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="23"/>
+    </row>
+    <row r="42" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="23"/>
-    </row>
-    <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="23"/>
+    </row>
+    <row r="43" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>42</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="23"/>
-    </row>
-    <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="23"/>
+    </row>
+    <row r="44" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="23"/>
-    </row>
-    <row r="45" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="23"/>
+    </row>
+    <row r="45" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>44</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="21"/>
-      <c r="J45" s="23"/>
-    </row>
-    <row r="46" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>116</v>
+      </c>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="23"/>
+    </row>
+    <row r="46" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="23"/>
-      <c r="J46" s="23"/>
-    </row>
-    <row r="47" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>46</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C47" s="6"/>
-    </row>
-    <row r="48" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C48" s="6"/>
+        <v>113</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="49" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>48</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C49" s="6"/>
+        <v>114</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C50" s="6"/>
+        <v>86</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C51" s="6"/>
+        <v>87</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="52" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="17"/>
-    </row>
-    <row r="53" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C53" s="6"/>
-      <c r="D53" s="23"/>
+        <v>94</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="54" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C54" s="6"/>
+        <v>95</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="55" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C55" s="6"/>
+        <v>121</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A56" s="5">
+        <v>55</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>123</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1688,6 +1848,7 @@
     <mergeCell ref="I35:I39"/>
     <mergeCell ref="I40:I45"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1696,7 +1857,7 @@
           <x14:formula1>
             <xm:f>Статусы!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C20 C21:C55</xm:sqref>
+          <xm:sqref>C2:C56</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1723,8 +1884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1AD7A76-A8AC-423F-98AB-A1F19B6CBDD3}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1760,32 +1921,32 @@
       <c r="B2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C2" s="20">
         <v>-5</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="27" t="s">
-        <v>72</v>
+      <c r="E2" s="24" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="27"/>
-    </row>
-    <row r="4" spans="1:5" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="24"/>
+    </row>
+    <row r="4" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
@@ -1798,7 +1959,7 @@
       <c r="D4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
@@ -1813,56 +1974,56 @@
       <c r="D5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="28" t="s">
-        <v>71</v>
+      <c r="E5" s="25" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="28"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="28"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="28"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" s="25"/>
+    </row>
+    <row r="9" spans="1:5" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>44</v>
       </c>
@@ -1875,99 +2036,99 @@
       <c r="D9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="28"/>
+      <c r="E9" s="25"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="24"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B12" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="24"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="17" t="s">
+      <c r="C13" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="24"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="18" t="s">
+      <c r="C14" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="27"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="17" t="s">
+      <c r="E14" s="24"/>
+    </row>
+    <row r="15" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>75</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="E12" s="27"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="E13" s="27"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="E14" s="27"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>78</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="27"/>
+        <v>84</v>
+      </c>
+      <c r="E15" s="24"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
@@ -1989,7 +2150,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2010,12 +2171,12 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>